<commit_message>
[IMP] {account,l10n}*_import: uniform way of importing matchings
The matching is now done in `account`, when posting, for all lines with
a matching number set to `I*` (where `*` can be anything)

task-3593885

closes odoo/enterprise#51027

X-original-commit: 718a9ef764431ea1ddf4b42d82c16c607b91599a
Related: odoo/upgrade#5372
Related: odoo/odoo#142691
Signed-off-by: Quentin De Paoli <qdp@odoo.com>
Signed-off-by: William André (wan) <wan@odoo.com>
</commit_message>
<xml_diff>
--- a/account_base_import/static/src/xls/journal_items_import.xlsx
+++ b/account_base_import/static/src/xls/journal_items_import.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t xml:space="preserve">journal_id</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matching_number</t>
   </si>
   <si>
     <t xml:space="preserve">MISC</t>
@@ -136,6 +139,18 @@
   </si>
   <si>
     <t xml:space="preserve">+++000/0000/05555+++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BNK1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BNK1/2021/00001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment</t>
   </si>
   <si>
     <t xml:space="preserve">(Optional) Import Journal Items</t>
@@ -522,37 +537,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -641,17 +625,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:V1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.81"/>
@@ -663,7 +647,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -688,7 +672,9 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4"/>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -705,22 +691,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>44536</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="7" t="n">
@@ -743,22 +729,22 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>44536</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="n">
@@ -781,22 +767,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>44536</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="7" t="n">
         <v>41750.89</v>
@@ -819,20 +805,20 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="8" t="n">
         <v>44531</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="n">
@@ -855,20 +841,20 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="8" t="n">
         <v>44531</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" s="6" t="n">
         <v>11750</v>
@@ -891,22 +877,22 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="8" t="n">
         <v>44531</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="7" t="n">
@@ -929,28 +915,30 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="8" t="n">
         <v>44531</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7" t="n">
         <v>11750</v>
       </c>
       <c r="H8" s="6"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -965,16 +953,32 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>44561</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="4"/>
+      <c r="H9" s="6" t="n">
+        <v>11750</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -989,14 +993,28 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="6"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>44561</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>11750</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -24586,8 +24604,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -24600,7 +24618,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -24609,10 +24627,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.77"/>
@@ -24649,7 +24667,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -24679,7 +24697,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -24710,10 +24728,10 @@
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -24742,10 +24760,10 @@
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="13" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -24774,10 +24792,10 @@
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="15" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -24806,10 +24824,10 @@
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
       <c r="B7" s="17" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -24838,7 +24856,7 @@
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="17" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -24871,7 +24889,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -24903,7 +24921,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -24932,10 +24950,10 @@
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="17" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -52354,8 +52372,8 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>